<commit_message>
Transactions - CRUD Accounts Only - CR
</commit_message>
<xml_diff>
--- a/docs/POC.xlsx
+++ b/docs/POC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TrackIT\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64420B5-54F1-4D5D-857C-218CE2AF338A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79942043-4E72-4CED-B06C-C29971D59C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{88A8090E-CF59-4DE3-A7B0-370C12A63438}"/>
   </bookViews>
@@ -18,10 +18,9 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Accounts!$A$1:$D$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Accounts!$A$1:$E$125</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="263">
   <si>
     <t>Accounts</t>
   </si>
@@ -818,6 +816,18 @@
   </si>
   <si>
     <t>2aba3b23-f2f4-f7e9-0c3d-7f68291ec0ee</t>
+  </si>
+  <si>
+    <t>transaction_type</t>
+  </si>
+  <si>
+    <t>Gift 1</t>
+  </si>
+  <si>
+    <t>a5c4ff6b-61e3-493d-8e11-4ccd006f557b</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
   </si>
 </sst>
 </file>
@@ -1187,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15335F2B-11FB-4D13-88B6-CE64AE69E9B3}">
-  <dimension ref="B2:K9"/>
+  <dimension ref="B2:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1202,16 +1212,17 @@
     <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -1225,12 +1236,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -1247,24 +1258,27 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
+        <v>259</v>
+      </c>
+      <c r="I6" t="s">
         <v>8</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>9</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>10</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>1</v>
       </c>
@@ -1291,21 +1305,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19178731-7566-4BD9-B588-0CF08FF1FE1F}">
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D41"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1313,13 +1328,16 @@
         <v>21</v>
       </c>
       <c r="C1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -1327,10 +1345,13 @@
         <v>132</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100000</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -1338,13 +1359,16 @@
         <v>126</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+        <v>101000</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -1352,13 +1376,16 @@
         <v>127</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+        <v>102000</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -1366,13 +1393,16 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+        <v>102001</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -1380,13 +1410,16 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+        <v>102002</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1394,13 +1427,16 @@
         <v>32</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
+        <v>102003</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -1408,13 +1444,16 @@
         <v>33</v>
       </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+        <v>102004</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -1422,13 +1461,16 @@
         <v>128</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+        <v>103000</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -1436,13 +1478,16 @@
         <v>34</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+        <v>103001</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -1450,13 +1495,16 @@
         <v>35</v>
       </c>
       <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
+        <v>103002</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -1464,13 +1512,16 @@
         <v>129</v>
       </c>
       <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+        <v>104000</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -1478,13 +1529,16 @@
         <v>36</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
+        <v>104001</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -1492,13 +1546,16 @@
         <v>37</v>
       </c>
       <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
+        <v>104002</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -1506,13 +1563,16 @@
         <v>38</v>
       </c>
       <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
+        <v>104003</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -1520,13 +1580,16 @@
         <v>39</v>
       </c>
       <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
+        <v>104004</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>151</v>
       </c>
@@ -1534,13 +1597,16 @@
         <v>40</v>
       </c>
       <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
+        <v>104005</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>152</v>
       </c>
@@ -1548,13 +1614,17 @@
         <v>41</v>
       </c>
       <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
+        <f>C17+1</f>
+        <v>104006</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>153</v>
       </c>
@@ -1562,13 +1632,17 @@
         <v>42</v>
       </c>
       <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
+        <f>C18+1</f>
+        <v>104007</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>154</v>
       </c>
@@ -1576,13 +1650,17 @@
         <v>43</v>
       </c>
       <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
+        <f>C19+1</f>
+        <v>104008</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -1590,13 +1668,17 @@
         <v>44</v>
       </c>
       <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
+        <f>C20+1</f>
+        <v>104009</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>156</v>
       </c>
@@ -1604,13 +1686,17 @@
         <v>45</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
+        <f>C21+1</f>
+        <v>104010</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>157</v>
       </c>
@@ -1618,10 +1704,13 @@
         <v>133</v>
       </c>
       <c r="C23">
+        <v>200000</v>
+      </c>
+      <c r="D23">
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>158</v>
       </c>
@@ -1629,13 +1718,16 @@
         <v>130</v>
       </c>
       <c r="C24">
+        <v>201000</v>
+      </c>
+      <c r="D24">
         <v>-1</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>159</v>
       </c>
@@ -1643,13 +1735,16 @@
         <v>46</v>
       </c>
       <c r="C25">
+        <v>201001</v>
+      </c>
+      <c r="D25">
         <v>-1</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>160</v>
       </c>
@@ -1657,13 +1752,16 @@
         <v>47</v>
       </c>
       <c r="C26">
+        <v>201002</v>
+      </c>
+      <c r="D26">
         <v>-1</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>161</v>
       </c>
@@ -1671,13 +1769,16 @@
         <v>131</v>
       </c>
       <c r="C27">
+        <v>202000</v>
+      </c>
+      <c r="D27">
         <v>-1</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>162</v>
       </c>
@@ -1685,13 +1786,16 @@
         <v>48</v>
       </c>
       <c r="C28">
+        <v>202001</v>
+      </c>
+      <c r="D28">
         <v>-1</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>163</v>
       </c>
@@ -1699,13 +1803,16 @@
         <v>49</v>
       </c>
       <c r="C29">
+        <v>202002</v>
+      </c>
+      <c r="D29">
         <v>-1</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -1713,10 +1820,13 @@
         <v>134</v>
       </c>
       <c r="C30">
+        <v>400000</v>
+      </c>
+      <c r="D30">
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>165</v>
       </c>
@@ -1724,13 +1834,16 @@
         <v>50</v>
       </c>
       <c r="C31">
+        <v>401000</v>
+      </c>
+      <c r="D31">
         <v>-1</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>166</v>
       </c>
@@ -1738,13 +1851,16 @@
         <v>50</v>
       </c>
       <c r="C32">
+        <v>401001</v>
+      </c>
+      <c r="D32">
         <v>-1</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>167</v>
       </c>
@@ -1752,13 +1868,16 @@
         <v>32</v>
       </c>
       <c r="C33">
+        <v>401002</v>
+      </c>
+      <c r="D33">
         <v>-1</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>168</v>
       </c>
@@ -1766,13 +1885,16 @@
         <v>51</v>
       </c>
       <c r="C34">
+        <v>401003</v>
+      </c>
+      <c r="D34">
         <v>-1</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>169</v>
       </c>
@@ -1780,13 +1902,16 @@
         <v>52</v>
       </c>
       <c r="C35">
+        <v>401004</v>
+      </c>
+      <c r="D35">
         <v>-1</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>170</v>
       </c>
@@ -1794,13 +1919,16 @@
         <v>53</v>
       </c>
       <c r="C36">
+        <v>402000</v>
+      </c>
+      <c r="D36">
         <v>-1</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>171</v>
       </c>
@@ -1808,13 +1936,16 @@
         <v>54</v>
       </c>
       <c r="C37">
+        <v>402001</v>
+      </c>
+      <c r="D37">
         <v>-1</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -1822,13 +1953,16 @@
         <v>55</v>
       </c>
       <c r="C38">
+        <v>402002</v>
+      </c>
+      <c r="D38">
         <v>-1</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>173</v>
       </c>
@@ -1836,13 +1970,16 @@
         <v>56</v>
       </c>
       <c r="C39">
+        <v>403000</v>
+      </c>
+      <c r="D39">
         <v>-1</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -1850,13 +1987,16 @@
         <v>67</v>
       </c>
       <c r="C40">
+        <v>404000</v>
+      </c>
+      <c r="D40">
         <v>-1</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>175</v>
       </c>
@@ -1864,10 +2004,13 @@
         <v>135</v>
       </c>
       <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>176</v>
       </c>
@@ -1875,13 +2018,16 @@
         <v>57</v>
       </c>
       <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
+        <v>501000</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>177</v>
       </c>
@@ -1889,13 +2035,16 @@
         <v>58</v>
       </c>
       <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
+        <v>501001</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>178</v>
       </c>
@@ -1903,13 +2052,16 @@
         <v>59</v>
       </c>
       <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
+        <v>501002</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>179</v>
       </c>
@@ -1917,13 +2069,16 @@
         <v>60</v>
       </c>
       <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
+        <v>501004</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>180</v>
       </c>
@@ -1931,13 +2086,16 @@
         <v>61</v>
       </c>
       <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
+        <v>501005</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>181</v>
       </c>
@@ -1945,13 +2103,16 @@
         <v>62</v>
       </c>
       <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
+        <v>501006</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>182</v>
       </c>
@@ -1959,13 +2120,16 @@
         <v>63</v>
       </c>
       <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
+        <v>501007</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>183</v>
       </c>
@@ -1973,13 +2137,16 @@
         <v>113</v>
       </c>
       <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
+        <v>501008</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>184</v>
       </c>
@@ -1987,13 +2154,16 @@
         <v>64</v>
       </c>
       <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
+        <v>502000</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>185</v>
       </c>
@@ -2001,13 +2171,16 @@
         <v>65</v>
       </c>
       <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
+        <v>502001</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>186</v>
       </c>
@@ -2015,13 +2188,16 @@
         <v>66</v>
       </c>
       <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
+        <v>502002</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>187</v>
       </c>
@@ -2029,13 +2205,16 @@
         <v>67</v>
       </c>
       <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
+        <v>502003</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>188</v>
       </c>
@@ -2043,13 +2222,16 @@
         <v>68</v>
       </c>
       <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
+        <v>503000</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>189</v>
       </c>
@@ -2057,13 +2239,16 @@
         <v>69</v>
       </c>
       <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55" t="s">
+        <v>503001</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>190</v>
       </c>
@@ -2071,13 +2256,16 @@
         <v>70</v>
       </c>
       <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
+        <v>504000</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>191</v>
       </c>
@@ -2085,13 +2273,16 @@
         <v>71</v>
       </c>
       <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
+        <v>504001</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>192</v>
       </c>
@@ -2099,13 +2290,16 @@
         <v>125</v>
       </c>
       <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58" t="s">
+        <v>504002</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>193</v>
       </c>
@@ -2113,13 +2307,16 @@
         <v>72</v>
       </c>
       <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59" t="s">
+        <v>504003</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>194</v>
       </c>
@@ -2127,13 +2324,16 @@
         <v>73</v>
       </c>
       <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60" t="s">
+        <v>504005</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>195</v>
       </c>
@@ -2141,13 +2341,16 @@
         <v>74</v>
       </c>
       <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61" t="s">
+        <v>505000</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>196</v>
       </c>
@@ -2155,13 +2358,16 @@
         <v>75</v>
       </c>
       <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62" t="s">
+        <v>505001</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>197</v>
       </c>
@@ -2169,13 +2375,16 @@
         <v>76</v>
       </c>
       <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63" t="s">
+        <v>505002</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>198</v>
       </c>
@@ -2183,13 +2392,16 @@
         <v>77</v>
       </c>
       <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="D64" t="s">
+        <v>505003</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>199</v>
       </c>
@@ -2197,13 +2409,16 @@
         <v>78</v>
       </c>
       <c r="C65">
-        <v>1</v>
-      </c>
-      <c r="D65" t="s">
+        <v>505004</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>200</v>
       </c>
@@ -2211,13 +2426,16 @@
         <v>79</v>
       </c>
       <c r="C66">
-        <v>1</v>
-      </c>
-      <c r="D66" t="s">
+        <v>505005</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>201</v>
       </c>
@@ -2225,13 +2443,16 @@
         <v>80</v>
       </c>
       <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67" t="s">
+        <v>506000</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>202</v>
       </c>
@@ -2239,13 +2460,16 @@
         <v>81</v>
       </c>
       <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="D68" t="s">
+        <v>506001</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>203</v>
       </c>
@@ -2253,13 +2477,16 @@
         <v>82</v>
       </c>
       <c r="C69">
-        <v>1</v>
-      </c>
-      <c r="D69" t="s">
+        <v>506002</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>204</v>
       </c>
@@ -2267,13 +2494,16 @@
         <v>83</v>
       </c>
       <c r="C70">
-        <v>1</v>
-      </c>
-      <c r="D70" t="s">
+        <v>506003</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>205</v>
       </c>
@@ -2281,13 +2511,16 @@
         <v>84</v>
       </c>
       <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71" t="s">
+        <v>506004</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>206</v>
       </c>
@@ -2295,13 +2528,16 @@
         <v>85</v>
       </c>
       <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72" t="s">
+        <v>507000</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>207</v>
       </c>
@@ -2309,13 +2545,16 @@
         <v>86</v>
       </c>
       <c r="C73">
-        <v>1</v>
-      </c>
-      <c r="D73" t="s">
+        <v>507001</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>208</v>
       </c>
@@ -2323,13 +2562,16 @@
         <v>87</v>
       </c>
       <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74" t="s">
+        <v>507002</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>209</v>
       </c>
@@ -2337,13 +2579,16 @@
         <v>88</v>
       </c>
       <c r="C75">
-        <v>1</v>
-      </c>
-      <c r="D75" t="s">
+        <v>507003</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>210</v>
       </c>
@@ -2351,13 +2596,16 @@
         <v>89</v>
       </c>
       <c r="C76">
-        <v>1</v>
-      </c>
-      <c r="D76" t="s">
+        <v>507004</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>211</v>
       </c>
@@ -2365,13 +2613,16 @@
         <v>85</v>
       </c>
       <c r="C77">
-        <v>1</v>
-      </c>
-      <c r="D77" t="s">
+        <v>507005</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>212</v>
       </c>
@@ -2379,13 +2630,16 @@
         <v>90</v>
       </c>
       <c r="C78">
-        <v>1</v>
-      </c>
-      <c r="D78" t="s">
+        <v>507006</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>213</v>
       </c>
@@ -2393,13 +2647,16 @@
         <v>91</v>
       </c>
       <c r="C79">
-        <v>1</v>
-      </c>
-      <c r="D79" t="s">
+        <v>508000</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>214</v>
       </c>
@@ -2407,13 +2664,16 @@
         <v>92</v>
       </c>
       <c r="C80">
-        <v>1</v>
-      </c>
-      <c r="D80" t="s">
+        <v>508002</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>215</v>
       </c>
@@ -2421,13 +2681,16 @@
         <v>93</v>
       </c>
       <c r="C81">
-        <v>1</v>
-      </c>
-      <c r="D81" t="s">
+        <v>508003</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>216</v>
       </c>
@@ -2435,13 +2698,16 @@
         <v>94</v>
       </c>
       <c r="C82">
-        <v>1</v>
-      </c>
-      <c r="D82" t="s">
+        <v>509000</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>217</v>
       </c>
@@ -2449,13 +2715,16 @@
         <v>95</v>
       </c>
       <c r="C83">
-        <v>1</v>
-      </c>
-      <c r="D83" t="s">
+        <v>509001</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>218</v>
       </c>
@@ -2463,13 +2732,16 @@
         <v>96</v>
       </c>
       <c r="C84">
-        <v>1</v>
-      </c>
-      <c r="D84" t="s">
+        <v>509002</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>219</v>
       </c>
@@ -2477,13 +2749,16 @@
         <v>97</v>
       </c>
       <c r="C85">
-        <v>1</v>
-      </c>
-      <c r="D85" t="s">
+        <v>509003</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>220</v>
       </c>
@@ -2491,546 +2766,680 @@
         <v>98</v>
       </c>
       <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86" t="s">
+        <v>510000</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>261</v>
+      </c>
+      <c r="B87" t="s">
+        <v>260</v>
+      </c>
+      <c r="C87">
+        <v>510001</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>221</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>53</v>
       </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="C88">
+        <v>511000</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>222</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>99</v>
       </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="C89">
+        <v>512000</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>223</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>100</v>
       </c>
-      <c r="C89">
-        <v>1</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="C90">
+        <v>512001</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>224</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>48</v>
       </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="C91">
+        <v>513000</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>225</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>101</v>
       </c>
-      <c r="C91">
-        <v>1</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="C92">
+        <v>513001</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>226</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>102</v>
       </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="C93">
+        <v>513002</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>227</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>103</v>
       </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="C94">
+        <v>513003</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>228</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>104</v>
       </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="C95">
+        <v>513004</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>229</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>105</v>
       </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="C96">
+        <v>513005</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>230</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>106</v>
       </c>
-      <c r="C96">
-        <v>1</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="C97">
+        <v>514000</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>231</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>107</v>
       </c>
-      <c r="C97">
-        <v>1</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="C98">
+        <v>514001</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>232</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>108</v>
       </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="C99">
+        <v>514002</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>233</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>104</v>
       </c>
-      <c r="C99">
-        <v>1</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="C100">
+        <v>514003</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>234</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>109</v>
       </c>
-      <c r="C100">
-        <v>1</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="C101">
+        <v>515000</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>235</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>110</v>
       </c>
-      <c r="C101">
-        <v>1</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="C102">
+        <v>515001</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>236</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>111</v>
       </c>
-      <c r="C102">
-        <v>1</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="C103">
+        <v>515002</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>237</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>104</v>
       </c>
-      <c r="C103">
-        <v>1</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="C104">
+        <v>515003</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>238</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>112</v>
       </c>
-      <c r="C104">
-        <v>1</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="C105">
+        <v>516000</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>239</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>101</v>
       </c>
-      <c r="C105">
-        <v>1</v>
-      </c>
-      <c r="D105" t="s">
+      <c r="C106">
+        <v>516001</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>240</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>102</v>
       </c>
-      <c r="C106">
-        <v>1</v>
-      </c>
-      <c r="D106" t="s">
+      <c r="C107">
+        <v>516002</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>241</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>104</v>
       </c>
-      <c r="C107">
-        <v>1</v>
-      </c>
-      <c r="D107" t="s">
+      <c r="C108">
+        <v>516003</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>242</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>105</v>
       </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="C109">
+        <v>516004</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>243</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>32</v>
       </c>
-      <c r="C109">
-        <v>1</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="C110">
+        <v>517000</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>244</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>114</v>
       </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="C111">
+        <v>517002</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>245</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>115</v>
       </c>
-      <c r="C111">
-        <v>1</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="C112">
+        <v>518000</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>246</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>116</v>
       </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="C113">
+        <v>518001</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>247</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>117</v>
       </c>
-      <c r="C113">
-        <v>1</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="C114">
+        <v>518002</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>248</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>118</v>
       </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-      <c r="D114" t="s">
+      <c r="C115">
+        <v>519000</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>249</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>119</v>
       </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="C116">
+        <v>519001</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>250</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>104</v>
       </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-      <c r="D116" t="s">
+      <c r="C117">
+        <v>519002</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>251</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B118" t="s">
         <v>120</v>
       </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
-      <c r="D117" t="s">
+      <c r="C118">
+        <v>520000</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>252</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B119" t="s">
         <v>101</v>
       </c>
-      <c r="C118">
-        <v>1</v>
-      </c>
-      <c r="D118" t="s">
+      <c r="C119">
+        <v>520001</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>253</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>121</v>
       </c>
-      <c r="C119">
-        <v>1</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="C120">
+        <v>520002</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>254</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B121" t="s">
         <v>122</v>
       </c>
-      <c r="C120">
-        <v>1</v>
-      </c>
-      <c r="D120" t="s">
+      <c r="C121">
+        <v>520003</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>255</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" t="s">
         <v>57</v>
       </c>
-      <c r="C121">
-        <v>1</v>
-      </c>
-      <c r="D121" t="s">
+      <c r="C122">
+        <v>520004</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>256</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>123</v>
       </c>
-      <c r="C122">
-        <v>1</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="C123">
+        <v>520005</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>257</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B124" t="s">
         <v>63</v>
       </c>
-      <c r="C123">
-        <v>1</v>
-      </c>
-      <c r="D123" t="s">
+      <c r="C124">
+        <v>520006</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>258</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" t="s">
         <v>124</v>
       </c>
-      <c r="C124">
-        <v>1</v>
-      </c>
-      <c r="D124" t="s">
+      <c r="C125">
+        <v>521000</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125" t="s">
         <v>175</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D124" xr:uid="{19178731-7566-4BD9-B588-0CF08FF1FE1F}"/>
+  <autoFilter ref="A1:E125" xr:uid="{19178731-7566-4BD9-B588-0CF08FF1FE1F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3039,8 +3448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB436D4-343E-4910-BF8F-8E0A55EC04EA}">
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A124" sqref="A2:C124"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>